<commit_message>
Increase Wikipedia pages used
</commit_message>
<xml_diff>
--- a/3-data/output/mpox_linked_pages_classified.xlsx
+++ b/3-data/output/mpox_linked_pages_classified.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/GitHub/mpox-wiki-analysis/3-data/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A550E1F-D685-C242-9E29-93859312B1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECE1B4B-8A83-934D-B425-F63DC74122B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4660" yWindow="-21100" windowWidth="18680" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4660" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$450</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1727,13 +1730,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" zoomScale="172" workbookViewId="0">
-      <selection activeCell="A401" sqref="A401"/>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2125,7 +2129,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2405,7 +2409,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -2717,7 +2721,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -3069,7 +3073,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
@@ -3085,7 +3089,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
@@ -3109,7 +3113,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
@@ -3117,7 +3121,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -3221,7 +3225,7 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
@@ -3285,7 +3289,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
@@ -3293,7 +3297,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
@@ -3301,7 +3305,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
@@ -3309,7 +3313,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
@@ -3357,7 +3361,7 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
@@ -3437,7 +3441,7 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
@@ -3645,7 +3649,7 @@
         <v>238</v>
       </c>
       <c r="B239">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
@@ -3957,7 +3961,7 @@
         <v>277</v>
       </c>
       <c r="B278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
@@ -4293,7 +4297,7 @@
         <v>319</v>
       </c>
       <c r="B320">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
@@ -4317,7 +4321,7 @@
         <v>322</v>
       </c>
       <c r="B323">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
@@ -4357,7 +4361,7 @@
         <v>327</v>
       </c>
       <c r="B328">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
@@ -4557,7 +4561,7 @@
         <v>352</v>
       </c>
       <c r="B353">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
@@ -4565,7 +4569,7 @@
         <v>353</v>
       </c>
       <c r="B354">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
@@ -4853,7 +4857,7 @@
         <v>389</v>
       </c>
       <c r="B390">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
@@ -4861,7 +4865,7 @@
         <v>390</v>
       </c>
       <c r="B391">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
@@ -5337,6 +5341,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B450" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>